<commit_message>
Minor adjustments to mappings
</commit_message>
<xml_diff>
--- a/Mappings/Alert - STU3.xlsx
+++ b/Mappings/Alert - STU3.xlsx
@@ -564,30 +564,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -897,7 +897,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -917,15 +917,15 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
       <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
@@ -938,16 +938,16 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="4"/>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="34"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="37"/>
       <c r="J2" s="5" t="s">
         <v>9</v>
       </c>
@@ -971,13 +971,13 @@
       <c r="I3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="35" t="s">
+      <c r="J3" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="K3" s="36" t="s">
+      <c r="K3" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="L3" s="37" t="s">
+      <c r="L3" s="31" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor edits in mappings xlsx files.
</commit_message>
<xml_diff>
--- a/Mappings/Alert - STU3.xlsx
+++ b/Mappings/Alert - STU3.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
   <si>
     <t xml:space="preserve"># </t>
   </si>
@@ -178,21 +178,6 @@
   </si>
   <si>
     <t>Flag.period.start</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Allowing a Condition reference: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>gForge trackerID 12798</t>
-    </r>
   </si>
   <si>
     <r>
@@ -234,6 +219,30 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> - Toevoegen EindDatum bij zibs die ook BeginDatum kennen.</t>
+    </r>
+  </si>
+  <si>
+    <t>De ZIB invariant verwijderen?</t>
+  </si>
+  <si>
+    <t>De valueset onder de loop laten nemen bij ZIB</t>
+  </si>
+  <si>
+    <t>Reference goed zetten</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Allowing a Condition reference: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>gForge trackerID 12798 - ZIB --&gt; ZIB-526</t>
     </r>
   </si>
 </sst>
@@ -894,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -913,7 +922,7 @@
     <col min="12" max="12" width="47.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -936,7 +945,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="A2" s="4"/>
       <c r="B2" s="34" t="s">
         <v>8</v>
@@ -953,7 +962,7 @@
       </c>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:12" ht="51.75">
+    <row r="3" spans="1:13" ht="51.75">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -978,10 +987,13 @@
         <v>51</v>
       </c>
       <c r="L3" s="31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="25.5">
+        <v>59</v>
+      </c>
+      <c r="M3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="25.5">
       <c r="A4" s="11">
         <v>2</v>
       </c>
@@ -1005,8 +1017,11 @@
       <c r="K4" s="26" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="L4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="11">
         <v>3</v>
       </c>
@@ -1029,7 +1044,7 @@
       </c>
       <c r="K5" s="27"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6" s="23">
         <v>4</v>
       </c>
@@ -1051,20 +1066,23 @@
         <v>48</v>
       </c>
       <c r="K6" s="28"/>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="L6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="L7" s="25" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="38.25">
+    <row r="8" spans="1:13" ht="38.25">
       <c r="L8" s="25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="25.5">
+      <c r="L9" s="25" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="25.5">
-      <c r="L9" s="25" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>